<commit_message>
Added lidar manufacturers, organized the folders
</commit_message>
<xml_diff>
--- a/Prototype Parts List.xlsx
+++ b/Prototype Parts List.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jancsi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jancsi\Documents\GitHub\VapnikAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF752AE1-6D48-44D8-A92E-0126C25CE1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ABD29E-4EB0-44D3-BC26-7714A8883C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{7E87D7F3-5FB9-492C-8434-7EFA8966433D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{7E87D7F3-5FB9-492C-8434-7EFA8966433D}"/>
   </bookViews>
   <sheets>
     <sheet name="Prototype V1.0" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="3" r:id="rId2"/>
+    <sheet name="LiDAR corps" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t>Component</t>
   </si>
@@ -220,6 +221,66 @@
   </si>
   <si>
     <t>MEMS, For true L4 at least 3</t>
+  </si>
+  <si>
+    <t>https://www.sick.com/be/en/detection-and-ranging-solutions/3d-lidar-sensors/c/g282752</t>
+  </si>
+  <si>
+    <t>SICK</t>
+  </si>
+  <si>
+    <t>https://leddartech.com/</t>
+  </si>
+  <si>
+    <t>Leddartech</t>
+  </si>
+  <si>
+    <t>https://quanergy.com/</t>
+  </si>
+  <si>
+    <t>Quanergy</t>
+  </si>
+  <si>
+    <t>https://www.robosense.ai/</t>
+  </si>
+  <si>
+    <t>Robosense</t>
+  </si>
+  <si>
+    <t>https://velodynelidar.com/</t>
+  </si>
+  <si>
+    <t>Velodyne</t>
+  </si>
+  <si>
+    <t>https://www.neuvition.com/</t>
+  </si>
+  <si>
+    <t>Neuvition</t>
+  </si>
+  <si>
+    <t>https://www.teledyneoptech.com/en/home/</t>
+  </si>
+  <si>
+    <t>Teledyne</t>
+  </si>
+  <si>
+    <t>https://www.zxlidars.com/</t>
+  </si>
+  <si>
+    <t>ZX LiDAR</t>
+  </si>
+  <si>
+    <t>https://www.aeye.ai/</t>
+  </si>
+  <si>
+    <t>Aeye</t>
+  </si>
+  <si>
+    <t>/+ System interators</t>
+  </si>
+  <si>
+    <t>https://www.continental-automotive.com/en-gl/Passenger-Cars/Autonomous-Mobility/Enablers/Lidars</t>
   </si>
 </sst>
 </file>
@@ -308,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -318,6 +379,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -639,13 +701,13 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="2" customWidth="1"/>
@@ -1293,8 +1355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B204B7A9-E759-4680-9001-3E7676790027}">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1403,7 @@
       <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D2">
@@ -2115,7 +2177,108 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" xr:uid="{CBD16C02-B822-46AD-BFC0-BB145137B8DC}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{60E07C68-B223-4079-953C-C4E566D8E902}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C570CB-1996-4DC8-9E5E-7C4256BE9687}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>